<commit_message>
Changed from survival to mortality in Shiny app (#4).
</commit_message>
<xml_diff>
--- a/shiny/texts.xlsx
+++ b/shiny/texts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHPR\Forskningsprojekt\Projekt 21-30\Projekt 29\shiny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\thamortpred\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C893900-3282-43AA-BC6F-4C6FC5F68603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="17364" yWindow="0" windowWidth="23796" windowHeight="20532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +42,6 @@
     <t>Do you have osteoarthritis of the hip? Do you consider a (cemented) total hip replacement? This is a secure and standardized procedure. The average risk to die within 90 days is 0.03 % in Sweden (3 deaths for every 10,000 patients). You can use this tool to get a more individualized estimate.</t>
   </si>
   <si>
-    <t>Your probability to survive at least 90 days is</t>
-  </si>
-  <si>
     <t>p_certainty_pre</t>
   </si>
   <si>
@@ -74,12 +72,6 @@
     <t>inte alltför långt ifrån</t>
   </si>
   <si>
-    <t>Din sannolikhet att överleva minst 90 dagar efter operationen ligger</t>
-  </si>
-  <si>
-    <t>90-day survival after total hip replacement</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -146,9 +138,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>90-dagarsöverlevnad efter insättning av höftprotes</t>
-  </si>
-  <si>
     <t>help_age_title</t>
   </si>
   <si>
@@ -206,9 +195,6 @@
     <t xml:space="preserve">Modellen vi använder baseras på registerdata där patienters kön identifierats via näst sista siffran i personnumret (dvs juridiskt kön). Vi har inte haft möjlighet att anpassa modellen efter annan könsidentitet. </t>
   </si>
   <si>
-    <t>Har du höftledsartros och överväger operation med en (cementerad) totalprotes? Detta är en standardiserad och väldigt säker operation. Av de som opereras i Sverige är det bara 0.03 % som avlider inom 90 dagar (dvs 3 av 10 000 patienter). Med ytterligare information kan vi ge en mer anpassad skattning för just din sannolikhet.</t>
-  </si>
-  <si>
     <t>&lt;p&gt; &lt;i&gt; Bedömning av ASA-klass görs av läkare i samband med operation som en grov skattning av generell hälsa. &lt;/i&gt;&lt;/p&gt; &lt;p&gt; &lt;b&gt;I = Normal hälsa. &lt;/b&gt; &lt;/p&gt; &lt;p&gt; &lt;b&gt; II = lindrig systemsjukdom* &lt;/b&gt; (t ex  aktiv rökare, regelbunden alkoholkonsumtion utan beroende eller missbruk, gravid, överviktig, välkontrollerad diabetes/högt blodtryck eller lindrig lungsjukdom. &lt;/p&gt; &lt;p&gt;  &lt;b&gt; III =  allvarlig systemsjukdom &lt;/b&gt; (t ex otillräckligt reglerad diabetes eller högt blodtryck, kronisk obstruktiv lungsjukdom [KOL],  sjuklig fetma, aktiv hepatit, alkoholberoende eller alkoholmissbruk, pacemakerberoende, måttligt  nedsatt ejektionsfraktion, ischemisk hjärtsjukdom, terminal njursvikt med regelbunden dialysbehandling, genomgången [&gt;3 månader] hjärtinfarkt eller  kranskärlsintervention, transitorisk ischemisk attack [TIA] eller stroke). &lt;/p&gt; &lt;p&gt; &lt;i&gt; * Texten är en generell översättning av instrumentet. T ex graviditet ska naturligtvis inte ses som sjukdom i någon vidare mening. &lt;/i&gt; &lt;/p&gt;</t>
   </si>
   <si>
@@ -260,16 +246,31 @@
     <t>Patients like you</t>
   </si>
   <si>
-    <t>Det behövs cirka &lt;b&gt; nnt &lt;/b&gt; patienter som dig för att en av dem ska dö inom 90 dagar efter operation. Det är dock fullt möjligt att denna patient skulle dö vid samma tidpunkt även utan att först ha opererat höften.</t>
-  </si>
-  <si>
     <t>It takes approximately &lt;b&gt; nnt &lt;/b&gt; patients like you for one of them to die within 90 days after surgery. It is possible however that this patient would have died at the same time regardless if he got operated or not.</t>
+  </si>
+  <si>
+    <t>Risk att dö inom 90-dagar efter insättning av höftprotes</t>
+  </si>
+  <si>
+    <t>Risk of death within 90-days after total hip replacement</t>
+  </si>
+  <si>
+    <t>Har du höftledsartros och överväger operation med en (cementerad) totalprotes? Detta är en standardiserad och väldigt säker operation. Av de som opereras i Sverige är det bara 0.03 % som avlider inom 90 dagar (dvs 3 av 10 000 patienter). Med ytterligare information kan vi ge en mer anpassad skattning för din sannolikhet.</t>
+  </si>
+  <si>
+    <t>Din risk att dö inom 90 dagar efter operationen ligger</t>
+  </si>
+  <si>
+    <t>Your risk to die within 90 days is</t>
+  </si>
+  <si>
+    <t>Det behövs cirka &lt;b&gt; nnt &lt;/b&gt; patienter som dig för att en av dem ska dö inom 90 dagar efter operation. Det är dock möjligt att denna patient skulle dött även utan en ny höft.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,21 +584,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="115.7109375" customWidth="1"/>
-    <col min="3" max="3" width="121.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115.6640625" customWidth="1"/>
+    <col min="3" max="3" width="121.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,290 +609,290 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B27" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C27" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Age distributuion. Fix #51.
</commit_message>
<xml_diff>
--- a/shiny/texts.xlsx
+++ b/shiny/texts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\thamortpred\shiny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHPR\Forskningsprojekt\Projekt 21-30\Projekt 29\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C893900-3282-43AA-BC6F-4C6FC5F68603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17364" yWindow="0" windowWidth="23796" windowHeight="20532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17364" yWindow="0" windowWidth="23796" windowHeight="20532"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,15 +146,9 @@
     <t>Age at surgery</t>
   </si>
   <si>
-    <t>How old will you be at the time of your planned hip replacement?</t>
-  </si>
-  <si>
     <t>Ålder vid operation</t>
   </si>
   <si>
-    <t>Hur gammal kommer du att vara vid den planerade operationen?</t>
-  </si>
-  <si>
     <t>help_sex_title</t>
   </si>
   <si>
@@ -265,12 +258,18 @@
   </si>
   <si>
     <t>Det behövs cirka &lt;b&gt; nnt &lt;/b&gt; patienter som dig för att en av dem ska dö inom 90 dagar efter operation. Det är dock möjligt att denna patient skulle dött även utan en ny höft.</t>
+  </si>
+  <si>
+    <t>Hur gammal kommer du att vara vid den planerade operationen? &lt;p&gt; I vårt underliggande studiematerial var den yngste patienten som dog 57 år och den äldste 95 år. Vi har således inga tillförlitliga data för skattningar utanför detta intervall.</t>
+  </si>
+  <si>
+    <t>How old will you be at the time of your planned hip replacement? &lt;p&gt; The youngest and oldest patients who died in the study cohort were 57 and 95 years old. We are unable to provide estimtes outside this range.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,10 +613,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -625,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -636,10 +635,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -757,142 +756,142 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>